<commit_message>
fixed some bugs and added prediction table
</commit_message>
<xml_diff>
--- a/public/BaderAldean_Accounts.xlsx
+++ b/public/BaderAldean_Accounts.xlsx
@@ -90,7 +90,7 @@
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
-          <t>QaEsewK</t>
+          <t>crEVBCu</t>
         </is>
       </c>
     </row>
@@ -110,7 +110,7 @@
       </c>
       <c r="D3" s="0" t="inlineStr">
         <is>
-          <t>QFjYxuV</t>
+          <t>DzLQJXF</t>
         </is>
       </c>
     </row>
@@ -130,7 +130,7 @@
       </c>
       <c r="D4" s="0" t="inlineStr">
         <is>
-          <t>LWa3i3c</t>
+          <t>xwC6c09</t>
         </is>
       </c>
     </row>
@@ -150,7 +150,7 @@
       </c>
       <c r="D5" s="0" t="inlineStr">
         <is>
-          <t>i5ErVbY</t>
+          <t>D5xeCHW</t>
         </is>
       </c>
     </row>
@@ -170,7 +170,7 @@
       </c>
       <c r="D6" s="0" t="inlineStr">
         <is>
-          <t>22zUWtn</t>
+          <t>HXk81eY</t>
         </is>
       </c>
     </row>
@@ -190,7 +190,7 @@
       </c>
       <c r="D7" s="0" t="inlineStr">
         <is>
-          <t>i3QDzCM</t>
+          <t>BA3nyT4</t>
         </is>
       </c>
     </row>
@@ -210,7 +210,7 @@
       </c>
       <c r="D8" s="0" t="inlineStr">
         <is>
-          <t>374ffrM</t>
+          <t>qj7uAMD</t>
         </is>
       </c>
     </row>
@@ -230,7 +230,7 @@
       </c>
       <c r="D9" s="0" t="inlineStr">
         <is>
-          <t>n4uYKh6</t>
+          <t>Le17bMO</t>
         </is>
       </c>
     </row>
@@ -250,7 +250,7 @@
       </c>
       <c r="D10" s="0" t="inlineStr">
         <is>
-          <t>mSC1qGc</t>
+          <t>NdvO6NV</t>
         </is>
       </c>
     </row>
@@ -270,7 +270,7 @@
       </c>
       <c r="D11" s="0" t="inlineStr">
         <is>
-          <t>r38SYge</t>
+          <t>GwPMOZd</t>
         </is>
       </c>
     </row>
@@ -290,7 +290,7 @@
       </c>
       <c r="D12" s="0" t="inlineStr">
         <is>
-          <t>a5Pf2sK</t>
+          <t>uXZduwT</t>
         </is>
       </c>
     </row>
@@ -310,7 +310,7 @@
       </c>
       <c r="D13" s="0" t="inlineStr">
         <is>
-          <t>kQr6LdV</t>
+          <t>a8FQgNH</t>
         </is>
       </c>
     </row>
@@ -330,7 +330,7 @@
       </c>
       <c r="D14" s="0" t="inlineStr">
         <is>
-          <t>8H2bFpz</t>
+          <t>TFVst32</t>
         </is>
       </c>
     </row>
@@ -350,7 +350,7 @@
       </c>
       <c r="D15" s="0" t="inlineStr">
         <is>
-          <t>7pyJG59</t>
+          <t>AF9BVvx</t>
         </is>
       </c>
     </row>
@@ -370,7 +370,7 @@
       </c>
       <c r="D16" s="0" t="inlineStr">
         <is>
-          <t>vXdw6V0</t>
+          <t>IPialY3</t>
         </is>
       </c>
     </row>
@@ -390,7 +390,7 @@
       </c>
       <c r="D17" s="0" t="inlineStr">
         <is>
-          <t>BhjDvyf</t>
+          <t>qhz0yx8</t>
         </is>
       </c>
     </row>
@@ -410,7 +410,7 @@
       </c>
       <c r="D18" s="0" t="inlineStr">
         <is>
-          <t>Ewhsk9o</t>
+          <t>B2kSZUD</t>
         </is>
       </c>
     </row>
@@ -430,7 +430,7 @@
       </c>
       <c r="D19" s="0" t="inlineStr">
         <is>
-          <t>4rlUSZG</t>
+          <t>CUPusvA</t>
         </is>
       </c>
     </row>
@@ -450,7 +450,7 @@
       </c>
       <c r="D20" s="0" t="inlineStr">
         <is>
-          <t>LLjJCRG</t>
+          <t>28Z0y8V</t>
         </is>
       </c>
     </row>
@@ -470,7 +470,7 @@
       </c>
       <c r="D21" s="0" t="inlineStr">
         <is>
-          <t>Sryr0rl</t>
+          <t>vB9hiWd</t>
         </is>
       </c>
     </row>
@@ -490,7 +490,7 @@
       </c>
       <c r="D22" s="0" t="inlineStr">
         <is>
-          <t>cDV3Gsu</t>
+          <t>7C3b7XL</t>
         </is>
       </c>
     </row>
@@ -510,7 +510,7 @@
       </c>
       <c r="D23" s="0" t="inlineStr">
         <is>
-          <t>TSSbMCS</t>
+          <t>zCRPpAZ</t>
         </is>
       </c>
     </row>
@@ -530,7 +530,7 @@
       </c>
       <c r="D24" s="0" t="inlineStr">
         <is>
-          <t>0akrTCI</t>
+          <t>xKkY4x6</t>
         </is>
       </c>
     </row>
@@ -550,7 +550,7 @@
       </c>
       <c r="D25" s="0" t="inlineStr">
         <is>
-          <t>NlFhsf2</t>
+          <t>PwV5ONe</t>
         </is>
       </c>
     </row>
@@ -570,7 +570,7 @@
       </c>
       <c r="D26" s="0" t="inlineStr">
         <is>
-          <t>1m0LJtT</t>
+          <t>nrxXtoX</t>
         </is>
       </c>
     </row>
@@ -590,7 +590,7 @@
       </c>
       <c r="D27" s="0" t="inlineStr">
         <is>
-          <t>2z7583P</t>
+          <t>syS0VCN</t>
         </is>
       </c>
     </row>
@@ -610,7 +610,7 @@
       </c>
       <c r="D28" s="0" t="inlineStr">
         <is>
-          <t>o8ifzgs</t>
+          <t>WeFGbxw</t>
         </is>
       </c>
     </row>
@@ -630,7 +630,7 @@
       </c>
       <c r="D29" s="0" t="inlineStr">
         <is>
-          <t>J5JMd1l</t>
+          <t>4hivFRY</t>
         </is>
       </c>
     </row>
@@ -650,7 +650,7 @@
       </c>
       <c r="D30" s="0" t="inlineStr">
         <is>
-          <t>FmWdXmr</t>
+          <t>3dxpPOy</t>
         </is>
       </c>
     </row>
@@ -670,7 +670,7 @@
       </c>
       <c r="D31" s="0" t="inlineStr">
         <is>
-          <t>ci2kYNJ</t>
+          <t>JaXJJBK</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
ended  the image things and added some routes
</commit_message>
<xml_diff>
--- a/public/BaderAldean_Accounts.xlsx
+++ b/public/BaderAldean_Accounts.xlsx
@@ -90,7 +90,7 @@
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
-          <t>Hgf6TX3</t>
+          <t>ieFSsp3</t>
         </is>
       </c>
     </row>
@@ -110,7 +110,7 @@
       </c>
       <c r="D3" s="0" t="inlineStr">
         <is>
-          <t>JJhPwQt</t>
+          <t>Kmj9vwJ</t>
         </is>
       </c>
     </row>
@@ -130,7 +130,7 @@
       </c>
       <c r="D4" s="0" t="inlineStr">
         <is>
-          <t>4qe6qTY</t>
+          <t>1i1V7Pe</t>
         </is>
       </c>
     </row>
@@ -150,7 +150,7 @@
       </c>
       <c r="D5" s="0" t="inlineStr">
         <is>
-          <t>cS9digV</t>
+          <t>rw3yfK1</t>
         </is>
       </c>
     </row>
@@ -170,7 +170,7 @@
       </c>
       <c r="D6" s="0" t="inlineStr">
         <is>
-          <t>Krmcc4Z</t>
+          <t>PWQwDao</t>
         </is>
       </c>
     </row>
@@ -190,7 +190,7 @@
       </c>
       <c r="D7" s="0" t="inlineStr">
         <is>
-          <t>4DpwycI</t>
+          <t>be6dvf0</t>
         </is>
       </c>
     </row>
@@ -210,7 +210,7 @@
       </c>
       <c r="D8" s="0" t="inlineStr">
         <is>
-          <t>AeIQLGl</t>
+          <t>hDnYltE</t>
         </is>
       </c>
     </row>
@@ -230,7 +230,7 @@
       </c>
       <c r="D9" s="0" t="inlineStr">
         <is>
-          <t>AkEccgx</t>
+          <t>VqlpGeK</t>
         </is>
       </c>
     </row>
@@ -250,7 +250,7 @@
       </c>
       <c r="D10" s="0" t="inlineStr">
         <is>
-          <t>lyJ7BYC</t>
+          <t>nv9pgB2</t>
         </is>
       </c>
     </row>
@@ -270,7 +270,7 @@
       </c>
       <c r="D11" s="0" t="inlineStr">
         <is>
-          <t>GGH2ciy</t>
+          <t>1jcEQSN</t>
         </is>
       </c>
     </row>
@@ -290,7 +290,7 @@
       </c>
       <c r="D12" s="0" t="inlineStr">
         <is>
-          <t>MwNNTXg</t>
+          <t>tejD45z</t>
         </is>
       </c>
     </row>
@@ -310,7 +310,7 @@
       </c>
       <c r="D13" s="0" t="inlineStr">
         <is>
-          <t>coxV4Y5</t>
+          <t>tc3zGGJ</t>
         </is>
       </c>
     </row>
@@ -330,7 +330,7 @@
       </c>
       <c r="D14" s="0" t="inlineStr">
         <is>
-          <t>36ItBJ1</t>
+          <t>4H9J2Ld</t>
         </is>
       </c>
     </row>
@@ -350,7 +350,7 @@
       </c>
       <c r="D15" s="0" t="inlineStr">
         <is>
-          <t>grBP3yv</t>
+          <t>nzWSjIr</t>
         </is>
       </c>
     </row>
@@ -370,7 +370,7 @@
       </c>
       <c r="D16" s="0" t="inlineStr">
         <is>
-          <t>OpZtEJH</t>
+          <t>4m4xmnB</t>
         </is>
       </c>
     </row>
@@ -390,7 +390,7 @@
       </c>
       <c r="D17" s="0" t="inlineStr">
         <is>
-          <t>UfmPfOD</t>
+          <t>4gfCO70</t>
         </is>
       </c>
     </row>
@@ -410,7 +410,7 @@
       </c>
       <c r="D18" s="0" t="inlineStr">
         <is>
-          <t>iT2uAWr</t>
+          <t>adHaT4C</t>
         </is>
       </c>
     </row>
@@ -430,7 +430,7 @@
       </c>
       <c r="D19" s="0" t="inlineStr">
         <is>
-          <t>USSpMGw</t>
+          <t>sHBuJAm</t>
         </is>
       </c>
     </row>
@@ -450,7 +450,7 @@
       </c>
       <c r="D20" s="0" t="inlineStr">
         <is>
-          <t>sxSUOA4</t>
+          <t>4Vfbka7</t>
         </is>
       </c>
     </row>
@@ -470,7 +470,7 @@
       </c>
       <c r="D21" s="0" t="inlineStr">
         <is>
-          <t>RoheAGd</t>
+          <t>6BjEsGI</t>
         </is>
       </c>
     </row>
@@ -490,7 +490,7 @@
       </c>
       <c r="D22" s="0" t="inlineStr">
         <is>
-          <t>cw3H2BO</t>
+          <t>SRhWOjT</t>
         </is>
       </c>
     </row>
@@ -510,7 +510,7 @@
       </c>
       <c r="D23" s="0" t="inlineStr">
         <is>
-          <t>ug5dtG5</t>
+          <t>IpBWhcY</t>
         </is>
       </c>
     </row>
@@ -530,7 +530,7 @@
       </c>
       <c r="D24" s="0" t="inlineStr">
         <is>
-          <t>3xslftl</t>
+          <t>69U7n0v</t>
         </is>
       </c>
     </row>
@@ -550,7 +550,7 @@
       </c>
       <c r="D25" s="0" t="inlineStr">
         <is>
-          <t>bUXL81v</t>
+          <t>0JiZykn</t>
         </is>
       </c>
     </row>
@@ -570,7 +570,7 @@
       </c>
       <c r="D26" s="0" t="inlineStr">
         <is>
-          <t>1S2jSXR</t>
+          <t>h0Wmll2</t>
         </is>
       </c>
     </row>
@@ -590,7 +590,7 @@
       </c>
       <c r="D27" s="0" t="inlineStr">
         <is>
-          <t>fwuGpdr</t>
+          <t>4ejEnqL</t>
         </is>
       </c>
     </row>
@@ -610,7 +610,7 @@
       </c>
       <c r="D28" s="0" t="inlineStr">
         <is>
-          <t>plRCti2</t>
+          <t>EGccYU4</t>
         </is>
       </c>
     </row>
@@ -630,7 +630,7 @@
       </c>
       <c r="D29" s="0" t="inlineStr">
         <is>
-          <t>jaKI4BF</t>
+          <t>g72C1S7</t>
         </is>
       </c>
     </row>
@@ -650,7 +650,7 @@
       </c>
       <c r="D30" s="0" t="inlineStr">
         <is>
-          <t>Xo35UBf</t>
+          <t>asfU8rD</t>
         </is>
       </c>
     </row>
@@ -670,7 +670,7 @@
       </c>
       <c r="D31" s="0" t="inlineStr">
         <is>
-          <t>sjGtDpa</t>
+          <t>qkvO4lr</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
moved settings/constants into a config file and fixed the problem that was happening
</commit_message>
<xml_diff>
--- a/public/BaderAldean_Accounts.xlsx
+++ b/public/BaderAldean_Accounts.xlsx
@@ -90,7 +90,7 @@
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
-          <t>ieFSsp3</t>
+          <t>ZnQyx4P</t>
         </is>
       </c>
     </row>
@@ -110,7 +110,7 @@
       </c>
       <c r="D3" s="0" t="inlineStr">
         <is>
-          <t>Kmj9vwJ</t>
+          <t>AtfsIpl</t>
         </is>
       </c>
     </row>
@@ -130,7 +130,7 @@
       </c>
       <c r="D4" s="0" t="inlineStr">
         <is>
-          <t>1i1V7Pe</t>
+          <t>mpSzJv3</t>
         </is>
       </c>
     </row>
@@ -150,7 +150,7 @@
       </c>
       <c r="D5" s="0" t="inlineStr">
         <is>
-          <t>rw3yfK1</t>
+          <t>jCYAttN</t>
         </is>
       </c>
     </row>
@@ -170,7 +170,7 @@
       </c>
       <c r="D6" s="0" t="inlineStr">
         <is>
-          <t>PWQwDao</t>
+          <t>tgBpxYb</t>
         </is>
       </c>
     </row>
@@ -190,7 +190,7 @@
       </c>
       <c r="D7" s="0" t="inlineStr">
         <is>
-          <t>be6dvf0</t>
+          <t>RrICFED</t>
         </is>
       </c>
     </row>
@@ -200,7 +200,7 @@
       </c>
       <c r="B8" s="0" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C8" s="0" t="inlineStr">
@@ -210,7 +210,7 @@
       </c>
       <c r="D8" s="0" t="inlineStr">
         <is>
-          <t>hDnYltE</t>
+          <t>JQlQ9NZ</t>
         </is>
       </c>
     </row>
@@ -220,7 +220,7 @@
       </c>
       <c r="B9" s="0" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C9" s="0" t="inlineStr">
@@ -230,7 +230,7 @@
       </c>
       <c r="D9" s="0" t="inlineStr">
         <is>
-          <t>VqlpGeK</t>
+          <t>DqR6KB2</t>
         </is>
       </c>
     </row>
@@ -240,7 +240,7 @@
       </c>
       <c r="B10" s="0" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C10" s="0" t="inlineStr">
@@ -250,7 +250,7 @@
       </c>
       <c r="D10" s="0" t="inlineStr">
         <is>
-          <t>nv9pgB2</t>
+          <t>A941tdW</t>
         </is>
       </c>
     </row>
@@ -260,7 +260,7 @@
       </c>
       <c r="B11" s="0" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C11" s="0" t="inlineStr">
@@ -270,7 +270,7 @@
       </c>
       <c r="D11" s="0" t="inlineStr">
         <is>
-          <t>1jcEQSN</t>
+          <t>ejZr2dX</t>
         </is>
       </c>
     </row>
@@ -280,7 +280,7 @@
       </c>
       <c r="B12" s="0" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C12" s="0" t="inlineStr">
@@ -290,7 +290,7 @@
       </c>
       <c r="D12" s="0" t="inlineStr">
         <is>
-          <t>tejD45z</t>
+          <t>n4D3AXE</t>
         </is>
       </c>
     </row>
@@ -300,7 +300,7 @@
       </c>
       <c r="B13" s="0" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C13" s="0" t="inlineStr">
@@ -310,7 +310,7 @@
       </c>
       <c r="D13" s="0" t="inlineStr">
         <is>
-          <t>tc3zGGJ</t>
+          <t>JZ3mNbv</t>
         </is>
       </c>
     </row>
@@ -320,7 +320,7 @@
       </c>
       <c r="B14" s="0" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C14" s="0" t="inlineStr">
@@ -330,7 +330,7 @@
       </c>
       <c r="D14" s="0" t="inlineStr">
         <is>
-          <t>4H9J2Ld</t>
+          <t>TPFGN1T</t>
         </is>
       </c>
     </row>
@@ -340,7 +340,7 @@
       </c>
       <c r="B15" s="0" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C15" s="0" t="inlineStr">
@@ -350,7 +350,7 @@
       </c>
       <c r="D15" s="0" t="inlineStr">
         <is>
-          <t>nzWSjIr</t>
+          <t>rI1rheM</t>
         </is>
       </c>
     </row>
@@ -360,7 +360,7 @@
       </c>
       <c r="B16" s="0" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C16" s="0" t="inlineStr">
@@ -370,7 +370,7 @@
       </c>
       <c r="D16" s="0" t="inlineStr">
         <is>
-          <t>4m4xmnB</t>
+          <t>GemE5BE</t>
         </is>
       </c>
     </row>
@@ -380,7 +380,7 @@
       </c>
       <c r="B17" s="0" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C17" s="0" t="inlineStr">
@@ -390,7 +390,7 @@
       </c>
       <c r="D17" s="0" t="inlineStr">
         <is>
-          <t>4gfCO70</t>
+          <t>Cfj6HOb</t>
         </is>
       </c>
     </row>
@@ -400,7 +400,7 @@
       </c>
       <c r="B18" s="0" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C18" s="0" t="inlineStr">
@@ -410,7 +410,7 @@
       </c>
       <c r="D18" s="0" t="inlineStr">
         <is>
-          <t>adHaT4C</t>
+          <t>d6qU3j1</t>
         </is>
       </c>
     </row>
@@ -420,7 +420,7 @@
       </c>
       <c r="B19" s="0" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C19" s="0" t="inlineStr">
@@ -430,7 +430,7 @@
       </c>
       <c r="D19" s="0" t="inlineStr">
         <is>
-          <t>sHBuJAm</t>
+          <t>n0R7veo</t>
         </is>
       </c>
     </row>
@@ -440,7 +440,7 @@
       </c>
       <c r="B20" s="0" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C20" s="0" t="inlineStr">
@@ -450,7 +450,7 @@
       </c>
       <c r="D20" s="0" t="inlineStr">
         <is>
-          <t>4Vfbka7</t>
+          <t>MRfvbL0</t>
         </is>
       </c>
     </row>
@@ -460,7 +460,7 @@
       </c>
       <c r="B21" s="0" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C21" s="0" t="inlineStr">
@@ -470,7 +470,7 @@
       </c>
       <c r="D21" s="0" t="inlineStr">
         <is>
-          <t>6BjEsGI</t>
+          <t>XnDrjGb</t>
         </is>
       </c>
     </row>
@@ -480,7 +480,7 @@
       </c>
       <c r="B22" s="0" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C22" s="0" t="inlineStr">
@@ -490,7 +490,7 @@
       </c>
       <c r="D22" s="0" t="inlineStr">
         <is>
-          <t>SRhWOjT</t>
+          <t>OlJ8vrp</t>
         </is>
       </c>
     </row>
@@ -500,7 +500,7 @@
       </c>
       <c r="B23" s="0" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C23" s="0" t="inlineStr">
@@ -510,7 +510,7 @@
       </c>
       <c r="D23" s="0" t="inlineStr">
         <is>
-          <t>IpBWhcY</t>
+          <t>KqpF2OI</t>
         </is>
       </c>
     </row>
@@ -520,7 +520,7 @@
       </c>
       <c r="B24" s="0" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C24" s="0" t="inlineStr">
@@ -530,7 +530,7 @@
       </c>
       <c r="D24" s="0" t="inlineStr">
         <is>
-          <t>69U7n0v</t>
+          <t>AJB43FK</t>
         </is>
       </c>
     </row>
@@ -540,7 +540,7 @@
       </c>
       <c r="B25" s="0" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C25" s="0" t="inlineStr">
@@ -550,7 +550,7 @@
       </c>
       <c r="D25" s="0" t="inlineStr">
         <is>
-          <t>0JiZykn</t>
+          <t>Xm63qfG</t>
         </is>
       </c>
     </row>
@@ -560,7 +560,7 @@
       </c>
       <c r="B26" s="0" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C26" s="0" t="inlineStr">
@@ -570,7 +570,7 @@
       </c>
       <c r="D26" s="0" t="inlineStr">
         <is>
-          <t>h0Wmll2</t>
+          <t>CkoJR9C</t>
         </is>
       </c>
     </row>
@@ -580,7 +580,7 @@
       </c>
       <c r="B27" s="0" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C27" s="0" t="inlineStr">
@@ -590,7 +590,7 @@
       </c>
       <c r="D27" s="0" t="inlineStr">
         <is>
-          <t>4ejEnqL</t>
+          <t>CYflJNi</t>
         </is>
       </c>
     </row>
@@ -600,7 +600,7 @@
       </c>
       <c r="B28" s="0" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C28" s="0" t="inlineStr">
@@ -610,7 +610,7 @@
       </c>
       <c r="D28" s="0" t="inlineStr">
         <is>
-          <t>EGccYU4</t>
+          <t>kYDMPTY</t>
         </is>
       </c>
     </row>
@@ -620,7 +620,7 @@
       </c>
       <c r="B29" s="0" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C29" s="0" t="inlineStr">
@@ -630,7 +630,7 @@
       </c>
       <c r="D29" s="0" t="inlineStr">
         <is>
-          <t>g72C1S7</t>
+          <t>GajbI0k</t>
         </is>
       </c>
     </row>
@@ -640,7 +640,7 @@
       </c>
       <c r="B30" s="0" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C30" s="0" t="inlineStr">
@@ -650,7 +650,7 @@
       </c>
       <c r="D30" s="0" t="inlineStr">
         <is>
-          <t>asfU8rD</t>
+          <t>VYvG9Ai</t>
         </is>
       </c>
     </row>
@@ -660,7 +660,7 @@
       </c>
       <c r="B31" s="0" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C31" s="0" t="inlineStr">
@@ -670,7 +670,7 @@
       </c>
       <c r="D31" s="0" t="inlineStr">
         <is>
-          <t>qkvO4lr</t>
+          <t>1S59RT0</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed declare match route
</commit_message>
<xml_diff>
--- a/public/BaderAldean_Accounts.xlsx
+++ b/public/BaderAldean_Accounts.xlsx
@@ -90,7 +90,7 @@
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
-          <t>ZnQyx4P</t>
+          <t>2zfWuPq</t>
         </is>
       </c>
     </row>
@@ -110,7 +110,7 @@
       </c>
       <c r="D3" s="0" t="inlineStr">
         <is>
-          <t>AtfsIpl</t>
+          <t>H2keyrt</t>
         </is>
       </c>
     </row>
@@ -130,7 +130,7 @@
       </c>
       <c r="D4" s="0" t="inlineStr">
         <is>
-          <t>mpSzJv3</t>
+          <t>lMN4ZYH</t>
         </is>
       </c>
     </row>
@@ -150,7 +150,7 @@
       </c>
       <c r="D5" s="0" t="inlineStr">
         <is>
-          <t>jCYAttN</t>
+          <t>utm6nz1</t>
         </is>
       </c>
     </row>
@@ -170,7 +170,7 @@
       </c>
       <c r="D6" s="0" t="inlineStr">
         <is>
-          <t>tgBpxYb</t>
+          <t>FifDwaR</t>
         </is>
       </c>
     </row>
@@ -190,7 +190,7 @@
       </c>
       <c r="D7" s="0" t="inlineStr">
         <is>
-          <t>RrICFED</t>
+          <t>Wx5kjLY</t>
         </is>
       </c>
     </row>
@@ -210,7 +210,7 @@
       </c>
       <c r="D8" s="0" t="inlineStr">
         <is>
-          <t>JQlQ9NZ</t>
+          <t>IkB6Lzf</t>
         </is>
       </c>
     </row>
@@ -230,7 +230,7 @@
       </c>
       <c r="D9" s="0" t="inlineStr">
         <is>
-          <t>DqR6KB2</t>
+          <t>T0orWdn</t>
         </is>
       </c>
     </row>
@@ -250,7 +250,7 @@
       </c>
       <c r="D10" s="0" t="inlineStr">
         <is>
-          <t>A941tdW</t>
+          <t>8aofEAE</t>
         </is>
       </c>
     </row>
@@ -270,7 +270,7 @@
       </c>
       <c r="D11" s="0" t="inlineStr">
         <is>
-          <t>ejZr2dX</t>
+          <t>K7NVKG5</t>
         </is>
       </c>
     </row>
@@ -290,7 +290,7 @@
       </c>
       <c r="D12" s="0" t="inlineStr">
         <is>
-          <t>n4D3AXE</t>
+          <t>45UUO3R</t>
         </is>
       </c>
     </row>
@@ -310,7 +310,7 @@
       </c>
       <c r="D13" s="0" t="inlineStr">
         <is>
-          <t>JZ3mNbv</t>
+          <t>2uGatTG</t>
         </is>
       </c>
     </row>
@@ -330,7 +330,7 @@
       </c>
       <c r="D14" s="0" t="inlineStr">
         <is>
-          <t>TPFGN1T</t>
+          <t>8ObgPzL</t>
         </is>
       </c>
     </row>
@@ -350,7 +350,7 @@
       </c>
       <c r="D15" s="0" t="inlineStr">
         <is>
-          <t>rI1rheM</t>
+          <t>U1BWtcV</t>
         </is>
       </c>
     </row>
@@ -370,7 +370,7 @@
       </c>
       <c r="D16" s="0" t="inlineStr">
         <is>
-          <t>GemE5BE</t>
+          <t>XA7mfYE</t>
         </is>
       </c>
     </row>
@@ -390,7 +390,7 @@
       </c>
       <c r="D17" s="0" t="inlineStr">
         <is>
-          <t>Cfj6HOb</t>
+          <t>drvOaIq</t>
         </is>
       </c>
     </row>
@@ -410,7 +410,7 @@
       </c>
       <c r="D18" s="0" t="inlineStr">
         <is>
-          <t>d6qU3j1</t>
+          <t>BKHFfcj</t>
         </is>
       </c>
     </row>
@@ -430,7 +430,7 @@
       </c>
       <c r="D19" s="0" t="inlineStr">
         <is>
-          <t>n0R7veo</t>
+          <t>MqSKwt7</t>
         </is>
       </c>
     </row>
@@ -450,7 +450,7 @@
       </c>
       <c r="D20" s="0" t="inlineStr">
         <is>
-          <t>MRfvbL0</t>
+          <t>VuJQsyS</t>
         </is>
       </c>
     </row>
@@ -470,7 +470,7 @@
       </c>
       <c r="D21" s="0" t="inlineStr">
         <is>
-          <t>XnDrjGb</t>
+          <t>gGKCX71</t>
         </is>
       </c>
     </row>
@@ -490,7 +490,7 @@
       </c>
       <c r="D22" s="0" t="inlineStr">
         <is>
-          <t>OlJ8vrp</t>
+          <t>m4xtMvd</t>
         </is>
       </c>
     </row>
@@ -510,7 +510,7 @@
       </c>
       <c r="D23" s="0" t="inlineStr">
         <is>
-          <t>KqpF2OI</t>
+          <t>gxx6ZeU</t>
         </is>
       </c>
     </row>
@@ -530,7 +530,7 @@
       </c>
       <c r="D24" s="0" t="inlineStr">
         <is>
-          <t>AJB43FK</t>
+          <t>JeK5w0d</t>
         </is>
       </c>
     </row>
@@ -550,7 +550,7 @@
       </c>
       <c r="D25" s="0" t="inlineStr">
         <is>
-          <t>Xm63qfG</t>
+          <t>6ASes5c</t>
         </is>
       </c>
     </row>
@@ -570,7 +570,7 @@
       </c>
       <c r="D26" s="0" t="inlineStr">
         <is>
-          <t>CkoJR9C</t>
+          <t>03ucRkh</t>
         </is>
       </c>
     </row>
@@ -590,7 +590,7 @@
       </c>
       <c r="D27" s="0" t="inlineStr">
         <is>
-          <t>CYflJNi</t>
+          <t>W2kVi52</t>
         </is>
       </c>
     </row>
@@ -610,7 +610,7 @@
       </c>
       <c r="D28" s="0" t="inlineStr">
         <is>
-          <t>kYDMPTY</t>
+          <t>mV8JY1B</t>
         </is>
       </c>
     </row>
@@ -630,7 +630,7 @@
       </c>
       <c r="D29" s="0" t="inlineStr">
         <is>
-          <t>GajbI0k</t>
+          <t>AmeI6Ee</t>
         </is>
       </c>
     </row>
@@ -650,7 +650,7 @@
       </c>
       <c r="D30" s="0" t="inlineStr">
         <is>
-          <t>VYvG9Ai</t>
+          <t>DKC2trB</t>
         </is>
       </c>
     </row>
@@ -670,7 +670,7 @@
       </c>
       <c r="D31" s="0" t="inlineStr">
         <is>
-          <t>1S59RT0</t>
+          <t>qwlZOpn</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed a dump error
</commit_message>
<xml_diff>
--- a/public/BaderAldean_Accounts.xlsx
+++ b/public/BaderAldean_Accounts.xlsx
@@ -90,7 +90,7 @@
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
-          <t>PbMcD3N</t>
+          <t>E6heiLs</t>
         </is>
       </c>
     </row>
@@ -110,7 +110,7 @@
       </c>
       <c r="D3" s="0" t="inlineStr">
         <is>
-          <t>rzSILpY</t>
+          <t>HCz67vr</t>
         </is>
       </c>
     </row>
@@ -130,7 +130,7 @@
       </c>
       <c r="D4" s="0" t="inlineStr">
         <is>
-          <t>koASHd1</t>
+          <t>VQULTYp</t>
         </is>
       </c>
     </row>
@@ -150,7 +150,7 @@
       </c>
       <c r="D5" s="0" t="inlineStr">
         <is>
-          <t>f5CuXS2</t>
+          <t>47dWcMW</t>
         </is>
       </c>
     </row>
@@ -170,7 +170,7 @@
       </c>
       <c r="D6" s="0" t="inlineStr">
         <is>
-          <t>mT6c1fP</t>
+          <t>LO6VDaL</t>
         </is>
       </c>
     </row>
@@ -190,7 +190,7 @@
       </c>
       <c r="D7" s="0" t="inlineStr">
         <is>
-          <t>rHDwu69</t>
+          <t>tFIXHDy</t>
         </is>
       </c>
     </row>
@@ -210,7 +210,7 @@
       </c>
       <c r="D8" s="0" t="inlineStr">
         <is>
-          <t>lQRx40N</t>
+          <t>or5hkdJ</t>
         </is>
       </c>
     </row>
@@ -230,7 +230,7 @@
       </c>
       <c r="D9" s="0" t="inlineStr">
         <is>
-          <t>9HCSakx</t>
+          <t>rPT8s4K</t>
         </is>
       </c>
     </row>
@@ -250,7 +250,7 @@
       </c>
       <c r="D10" s="0" t="inlineStr">
         <is>
-          <t>mbP7KhW</t>
+          <t>asQNTwb</t>
         </is>
       </c>
     </row>
@@ -270,7 +270,7 @@
       </c>
       <c r="D11" s="0" t="inlineStr">
         <is>
-          <t>p0IbRjM</t>
+          <t>JPBuHoZ</t>
         </is>
       </c>
     </row>
@@ -290,7 +290,7 @@
       </c>
       <c r="D12" s="0" t="inlineStr">
         <is>
-          <t>juAI6NT</t>
+          <t>eF80d5y</t>
         </is>
       </c>
     </row>
@@ -310,7 +310,7 @@
       </c>
       <c r="D13" s="0" t="inlineStr">
         <is>
-          <t>r8XK5va</t>
+          <t>X7llUky</t>
         </is>
       </c>
     </row>
@@ -330,7 +330,7 @@
       </c>
       <c r="D14" s="0" t="inlineStr">
         <is>
-          <t>7gMsFnT</t>
+          <t>vcOBslO</t>
         </is>
       </c>
     </row>
@@ -350,7 +350,7 @@
       </c>
       <c r="D15" s="0" t="inlineStr">
         <is>
-          <t>nEt0SiC</t>
+          <t>z0hKsnc</t>
         </is>
       </c>
     </row>
@@ -370,7 +370,7 @@
       </c>
       <c r="D16" s="0" t="inlineStr">
         <is>
-          <t>ozMuyAG</t>
+          <t>XgztlEH</t>
         </is>
       </c>
     </row>
@@ -390,7 +390,7 @@
       </c>
       <c r="D17" s="0" t="inlineStr">
         <is>
-          <t>jDeZ5NI</t>
+          <t>iT6SeRU</t>
         </is>
       </c>
     </row>
@@ -410,7 +410,7 @@
       </c>
       <c r="D18" s="0" t="inlineStr">
         <is>
-          <t>ovNl9py</t>
+          <t>nTscjpp</t>
         </is>
       </c>
     </row>
@@ -430,7 +430,7 @@
       </c>
       <c r="D19" s="0" t="inlineStr">
         <is>
-          <t>XxhEnsk</t>
+          <t>wNecFKN</t>
         </is>
       </c>
     </row>
@@ -450,7 +450,7 @@
       </c>
       <c r="D20" s="0" t="inlineStr">
         <is>
-          <t>0hMK17Z</t>
+          <t>t4evQI0</t>
         </is>
       </c>
     </row>
@@ -470,7 +470,7 @@
       </c>
       <c r="D21" s="0" t="inlineStr">
         <is>
-          <t>SlS2FbT</t>
+          <t>upY07IW</t>
         </is>
       </c>
     </row>
@@ -490,7 +490,7 @@
       </c>
       <c r="D22" s="0" t="inlineStr">
         <is>
-          <t>Zzz4sXO</t>
+          <t>SXgPQsx</t>
         </is>
       </c>
     </row>
@@ -510,7 +510,7 @@
       </c>
       <c r="D23" s="0" t="inlineStr">
         <is>
-          <t>1VCxDet</t>
+          <t>n1mbLt9</t>
         </is>
       </c>
     </row>
@@ -530,7 +530,7 @@
       </c>
       <c r="D24" s="0" t="inlineStr">
         <is>
-          <t>tJPTKmx</t>
+          <t>4kiiGdm</t>
         </is>
       </c>
     </row>
@@ -550,7 +550,7 @@
       </c>
       <c r="D25" s="0" t="inlineStr">
         <is>
-          <t>1HbfEua</t>
+          <t>op0YXGv</t>
         </is>
       </c>
     </row>
@@ -570,7 +570,7 @@
       </c>
       <c r="D26" s="0" t="inlineStr">
         <is>
-          <t>8qZ2TgG</t>
+          <t>HKGdLbK</t>
         </is>
       </c>
     </row>
@@ -590,7 +590,7 @@
       </c>
       <c r="D27" s="0" t="inlineStr">
         <is>
-          <t>H7qIGYH</t>
+          <t>OVkbyQH</t>
         </is>
       </c>
     </row>
@@ -610,7 +610,7 @@
       </c>
       <c r="D28" s="0" t="inlineStr">
         <is>
-          <t>JV5f5R7</t>
+          <t>rSiTxyV</t>
         </is>
       </c>
     </row>
@@ -630,7 +630,7 @@
       </c>
       <c r="D29" s="0" t="inlineStr">
         <is>
-          <t>XSAeog1</t>
+          <t>0FYUwts</t>
         </is>
       </c>
     </row>
@@ -650,7 +650,7 @@
       </c>
       <c r="D30" s="0" t="inlineStr">
         <is>
-          <t>rLuTBe4</t>
+          <t>BogNRaD</t>
         </is>
       </c>
     </row>
@@ -670,7 +670,7 @@
       </c>
       <c r="D31" s="0" t="inlineStr">
         <is>
-          <t>sUfswpT</t>
+          <t>SWpJeTh</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added (delete match),added (add new match),changed (part 2 view teams),added (declare winners),changed( advance to part 2),settings(added 9 winnner and 7&8 winner)
</commit_message>
<xml_diff>
--- a/public/BaderAldean_Accounts.xlsx
+++ b/public/BaderAldean_Accounts.xlsx
@@ -90,7 +90,7 @@
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
-          <t>FKHWmga</t>
+          <t>csqSMKo</t>
         </is>
       </c>
     </row>
@@ -110,7 +110,7 @@
       </c>
       <c r="D3" s="0" t="inlineStr">
         <is>
-          <t>JGZxgKT</t>
+          <t>lKIjJgi</t>
         </is>
       </c>
     </row>
@@ -130,7 +130,7 @@
       </c>
       <c r="D4" s="0" t="inlineStr">
         <is>
-          <t>wPG9uxx</t>
+          <t>nuu6WVj</t>
         </is>
       </c>
     </row>
@@ -150,7 +150,7 @@
       </c>
       <c r="D5" s="0" t="inlineStr">
         <is>
-          <t>aYon9zY</t>
+          <t>gNlFrnA</t>
         </is>
       </c>
     </row>
@@ -170,7 +170,7 @@
       </c>
       <c r="D6" s="0" t="inlineStr">
         <is>
-          <t>kLrPWAR</t>
+          <t>kfjPBKb</t>
         </is>
       </c>
     </row>
@@ -190,7 +190,7 @@
       </c>
       <c r="D7" s="0" t="inlineStr">
         <is>
-          <t>TxMOVxd</t>
+          <t>fap2rBX</t>
         </is>
       </c>
     </row>
@@ -210,7 +210,7 @@
       </c>
       <c r="D8" s="0" t="inlineStr">
         <is>
-          <t>5tomI0m</t>
+          <t>HXi0QdJ</t>
         </is>
       </c>
     </row>
@@ -230,7 +230,7 @@
       </c>
       <c r="D9" s="0" t="inlineStr">
         <is>
-          <t>I6apssg</t>
+          <t>L7Iu4LE</t>
         </is>
       </c>
     </row>
@@ -250,7 +250,7 @@
       </c>
       <c r="D10" s="0" t="inlineStr">
         <is>
-          <t>E3K0TMN</t>
+          <t>8yKVBUY</t>
         </is>
       </c>
     </row>
@@ -270,7 +270,7 @@
       </c>
       <c r="D11" s="0" t="inlineStr">
         <is>
-          <t>531jmrj</t>
+          <t>GmIUkwk</t>
         </is>
       </c>
     </row>
@@ -290,7 +290,7 @@
       </c>
       <c r="D12" s="0" t="inlineStr">
         <is>
-          <t>oi1u5wn</t>
+          <t>ulrDs75</t>
         </is>
       </c>
     </row>
@@ -310,7 +310,7 @@
       </c>
       <c r="D13" s="0" t="inlineStr">
         <is>
-          <t>3QNz4Yg</t>
+          <t>9R0ZWgg</t>
         </is>
       </c>
     </row>
@@ -330,7 +330,7 @@
       </c>
       <c r="D14" s="0" t="inlineStr">
         <is>
-          <t>UEiXZA3</t>
+          <t>apkiWiv</t>
         </is>
       </c>
     </row>
@@ -350,7 +350,7 @@
       </c>
       <c r="D15" s="0" t="inlineStr">
         <is>
-          <t>w7t9t82</t>
+          <t>dbD3QC7</t>
         </is>
       </c>
     </row>
@@ -370,7 +370,7 @@
       </c>
       <c r="D16" s="0" t="inlineStr">
         <is>
-          <t>UXWQYQ0</t>
+          <t>2sizpzC</t>
         </is>
       </c>
     </row>
@@ -390,7 +390,7 @@
       </c>
       <c r="D17" s="0" t="inlineStr">
         <is>
-          <t>iAHbILY</t>
+          <t>Uen6vxf</t>
         </is>
       </c>
     </row>
@@ -410,7 +410,7 @@
       </c>
       <c r="D18" s="0" t="inlineStr">
         <is>
-          <t>bNH41wQ</t>
+          <t>nWpUXXj</t>
         </is>
       </c>
     </row>
@@ -430,7 +430,7 @@
       </c>
       <c r="D19" s="0" t="inlineStr">
         <is>
-          <t>f3fouHz</t>
+          <t>rzDXLo6</t>
         </is>
       </c>
     </row>
@@ -450,7 +450,7 @@
       </c>
       <c r="D20" s="0" t="inlineStr">
         <is>
-          <t>0NZq63g</t>
+          <t>6CSVdf9</t>
         </is>
       </c>
     </row>
@@ -470,7 +470,7 @@
       </c>
       <c r="D21" s="0" t="inlineStr">
         <is>
-          <t>0pOMVOC</t>
+          <t>Gj839oi</t>
         </is>
       </c>
     </row>
@@ -490,7 +490,7 @@
       </c>
       <c r="D22" s="0" t="inlineStr">
         <is>
-          <t>ZbYxUCb</t>
+          <t>ra6xDmi</t>
         </is>
       </c>
     </row>
@@ -510,7 +510,7 @@
       </c>
       <c r="D23" s="0" t="inlineStr">
         <is>
-          <t>mzJ3DlB</t>
+          <t>P3B81gb</t>
         </is>
       </c>
     </row>
@@ -530,7 +530,7 @@
       </c>
       <c r="D24" s="0" t="inlineStr">
         <is>
-          <t>lFjwyj9</t>
+          <t>hOSzRlj</t>
         </is>
       </c>
     </row>
@@ -550,7 +550,7 @@
       </c>
       <c r="D25" s="0" t="inlineStr">
         <is>
-          <t>SqIZsD4</t>
+          <t>h1Mbm4R</t>
         </is>
       </c>
     </row>
@@ -570,7 +570,7 @@
       </c>
       <c r="D26" s="0" t="inlineStr">
         <is>
-          <t>LbzvxKJ</t>
+          <t>BQHlAP2</t>
         </is>
       </c>
     </row>
@@ -590,7 +590,7 @@
       </c>
       <c r="D27" s="0" t="inlineStr">
         <is>
-          <t>zi2hD18</t>
+          <t>rSW4ELP</t>
         </is>
       </c>
     </row>
@@ -610,7 +610,7 @@
       </c>
       <c r="D28" s="0" t="inlineStr">
         <is>
-          <t>3ndbqNH</t>
+          <t>IHoIARd</t>
         </is>
       </c>
     </row>
@@ -630,7 +630,7 @@
       </c>
       <c r="D29" s="0" t="inlineStr">
         <is>
-          <t>fQU2fnr</t>
+          <t>bLZkhhx</t>
         </is>
       </c>
     </row>
@@ -650,7 +650,7 @@
       </c>
       <c r="D30" s="0" t="inlineStr">
         <is>
-          <t>9nOqCd2</t>
+          <t>lavm8P4</t>
         </is>
       </c>
     </row>
@@ -670,7 +670,607 @@
       </c>
       <c r="D31" s="0" t="inlineStr">
         <is>
-          <t>xOZBzaX</t>
+          <t>28xNgVg</t>
+        </is>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="0">
+        <v>9</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>captain A9</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>KonOoL3</t>
+        </is>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="0">
+        <v>9</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>keeper A9</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>OCkg9ir</t>
+        </is>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="0">
+        <v>9</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>3A9</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>0wDUR8v</t>
+        </is>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="0">
+        <v>9</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>4A9</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>XOQvvRL</t>
+        </is>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="0">
+        <v>9</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>5A9</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>zggN3ge</t>
+        </is>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="0">
+        <v>9</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>6A9</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>5HovYyF</t>
+        </is>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="0">
+        <v>9</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>captain B9</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>OfLaznw</t>
+        </is>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="0">
+        <v>9</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>keeper B9</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>ek711nj</t>
+        </is>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="0">
+        <v>9</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>3B9</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>DfSCnI1</t>
+        </is>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="0">
+        <v>9</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>4B9</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>eCCRBqZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="0">
+        <v>9</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>5B9</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>JFQvpGs</t>
+        </is>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="0">
+        <v>9</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>6B9</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>B3fmfts</t>
+        </is>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="0">
+        <v>9</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>captain C9</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>rpj5bKa</t>
+        </is>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="0">
+        <v>9</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>keeper C9</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>JSINnkg</t>
+        </is>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="0">
+        <v>9</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>3C9</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>Wd15r22</t>
+        </is>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="0">
+        <v>9</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>4C9</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>mqbBCqy</t>
+        </is>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="0">
+        <v>9</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>5C9</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>e5dgbOk</t>
+        </is>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="0">
+        <v>9</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>6C9</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>rdfsVhC</t>
+        </is>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="0">
+        <v>9</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>captain D9</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>J7GNjfV</t>
+        </is>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="0">
+        <v>9</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>keeper D9</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>xHXD0c8</t>
+        </is>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="0">
+        <v>9</v>
+      </c>
+      <c r="B52" s="0" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C52" s="0" t="inlineStr">
+        <is>
+          <t>3D9</t>
+        </is>
+      </c>
+      <c r="D52" s="0" t="inlineStr">
+        <is>
+          <t>m77la8m</t>
+        </is>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="0">
+        <v>9</v>
+      </c>
+      <c r="B53" s="0" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C53" s="0" t="inlineStr">
+        <is>
+          <t>4D9</t>
+        </is>
+      </c>
+      <c r="D53" s="0" t="inlineStr">
+        <is>
+          <t>E1iCRvj</t>
+        </is>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="0">
+        <v>9</v>
+      </c>
+      <c r="B54" s="0" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C54" s="0" t="inlineStr">
+        <is>
+          <t>5D9</t>
+        </is>
+      </c>
+      <c r="D54" s="0" t="inlineStr">
+        <is>
+          <t>XOqi5qt</t>
+        </is>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="0">
+        <v>9</v>
+      </c>
+      <c r="B55" s="0" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C55" s="0" t="inlineStr">
+        <is>
+          <t>6D9</t>
+        </is>
+      </c>
+      <c r="D55" s="0" t="inlineStr">
+        <is>
+          <t>64ckujW</t>
+        </is>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="0">
+        <v>9</v>
+      </c>
+      <c r="B56" s="0" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C56" s="0" t="inlineStr">
+        <is>
+          <t>captain E9</t>
+        </is>
+      </c>
+      <c r="D56" s="0" t="inlineStr">
+        <is>
+          <t>FjhWZKF</t>
+        </is>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="0">
+        <v>9</v>
+      </c>
+      <c r="B57" s="0" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C57" s="0" t="inlineStr">
+        <is>
+          <t>keeper E9</t>
+        </is>
+      </c>
+      <c r="D57" s="0" t="inlineStr">
+        <is>
+          <t>YEMKM6s</t>
+        </is>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="0">
+        <v>9</v>
+      </c>
+      <c r="B58" s="0" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C58" s="0" t="inlineStr">
+        <is>
+          <t>3\e9</t>
+        </is>
+      </c>
+      <c r="D58" s="0" t="inlineStr">
+        <is>
+          <t>2BcuqOm</t>
+        </is>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="0">
+        <v>9</v>
+      </c>
+      <c r="B59" s="0" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C59" s="0" t="inlineStr">
+        <is>
+          <t>4\E9</t>
+        </is>
+      </c>
+      <c r="D59" s="0" t="inlineStr">
+        <is>
+          <t>umH3ErF</t>
+        </is>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="0">
+        <v>9</v>
+      </c>
+      <c r="B60" s="0" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C60" s="0" t="inlineStr">
+        <is>
+          <t>5E\9</t>
+        </is>
+      </c>
+      <c r="D60" s="0" t="inlineStr">
+        <is>
+          <t>VjyLmUF</t>
+        </is>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="0">
+        <v>9</v>
+      </c>
+      <c r="B61" s="0" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C61" s="0" t="inlineStr">
+        <is>
+          <t>6E/9</t>
+        </is>
+      </c>
+      <c r="D61" s="0" t="inlineStr">
+        <is>
+          <t>E84mbF6</t>
         </is>
       </c>
     </row>

</xml_diff>